<commit_message>
Rencana penyusunan bukti kelengkapan
</commit_message>
<xml_diff>
--- a/Arsitektur Sistem.xlsx
+++ b/Arsitektur Sistem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\lsp_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811F9333-0DE7-4CB3-BCCE-73B9F36A8B1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B32D6E-7305-4817-9485-C672CE3378B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="24000" windowHeight="9740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="85">
   <si>
     <t>NAMA ID</t>
   </si>
@@ -271,6 +271,30 @@
   </si>
   <si>
     <t>satuData_kuk</t>
+  </si>
+  <si>
+    <t>id_form_bukti</t>
+  </si>
+  <si>
+    <t>Bukti Kelengkapan</t>
+  </si>
+  <si>
+    <t>Asesi</t>
+  </si>
+  <si>
+    <t>id_tabel_bukti</t>
+  </si>
+  <si>
+    <t>id_modal_form_bukti</t>
+  </si>
+  <si>
+    <t>datatabel_bukti</t>
+  </si>
+  <si>
+    <t>form_bukti</t>
+  </si>
+  <si>
+    <t>satuData_bukti</t>
   </si>
 </sst>
 </file>
@@ -607,10 +631,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,6 +745,17 @@
       </c>
       <c r="D9" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -777,10 +812,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,6 +950,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -925,10 +971,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,6 +1096,17 @@
       </c>
       <c r="D10" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1123,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1136,10 +1193,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1274,6 +1331,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1284,10 +1352,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1367,6 +1435,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1377,10 +1456,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1459,6 +1538,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1469,10 +1559,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1749,6 +1839,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1759,10 +1871,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1852,6 +1964,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>